<commit_message>
CSV auskommentiert Kosmetische anpassungen Excel Template angepasst
</commit_message>
<xml_diff>
--- a/backend/templates/fahrtenabrechnung_vorlage.xlsx
+++ b/backend/templates/fahrtenabrechnung_vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonluthe/Documents/Fahrtenbuch/backend/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC137C6-20FB-C446-B1C4-DA7C31A97C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F561D8-F62F-2547-B80B-3CE26E080A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{F46B887E-D2C8-3347-9EF3-8F9C6453CC26}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" xr2:uid="{F46B887E-D2C8-3347-9EF3-8F9C6453CC26}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>km x 0,30 € =</t>
-  </si>
-  <si>
-    <t>€</t>
   </si>
   <si>
     <t>Angaben zur mitgenommenen Person</t>
@@ -278,18 +275,6 @@
   </si>
   <si>
     <t>Datum: _________________________</t>
-  </si>
-  <si>
-    <t>Kirchengemeinde Wesselburen</t>
-  </si>
-  <si>
-    <t>Pastor Simon Luthe</t>
-  </si>
-  <si>
-    <t>Süderstr. 18, 25779 Hennstedt</t>
-  </si>
-  <si>
-    <t>DE90214500000105491377</t>
   </si>
 </sst>
 </file>
@@ -926,7 +911,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1119,6 +1104,12 @@
     <xf numFmtId="8" fontId="11" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1137,79 +1128,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -1218,8 +1136,74 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1533,8 +1517,8 @@
   </sheetPr>
   <dimension ref="A3:J22"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1553,7 +1537,7 @@
   <sheetData>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="35"/>
       <c r="E3" s="3"/>
@@ -1567,7 +1551,7 @@
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
@@ -1586,11 +1570,9 @@
         <v>5</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="36" t="s">
-        <v>45</v>
-      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -1605,43 +1587,37 @@
         <v>6</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="104" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
     </row>
     <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="106" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="102" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -1655,7 +1631,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -1669,17 +1645,17 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1710,7 +1686,7 @@
   </sheetPr>
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H19" sqref="H19:J19"/>
     </sheetView>
   </sheetViews>
@@ -1735,7 +1711,7 @@
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="49"/>
@@ -1744,9 +1720,9 @@
       <c r="F2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="53" t="str">
+      <c r="G2" s="53">
         <f>Vorlage!C11</f>
-        <v>Pastor Simon Luthe</v>
+        <v>0</v>
       </c>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
@@ -1757,9 +1733,9 @@
       <c r="A3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="56" t="str">
+      <c r="B3" s="56">
         <f>Vorlage!C7</f>
-        <v>Kirchengemeinde Wesselburen</v>
+        <v>0</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="41"/>
@@ -1767,9 +1743,9 @@
       <c r="F3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="59" t="str">
+      <c r="G3" s="59">
         <f>Vorlage!C12</f>
-        <v>Süderstr. 18, 25779 Hennstedt</v>
+        <v>0</v>
       </c>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
@@ -1785,16 +1761,16 @@
       <c r="D4" s="62"/>
       <c r="E4" s="62"/>
       <c r="F4" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="43" t="str">
+        <v>23</v>
+      </c>
+      <c r="G4" s="43">
         <f>Vorlage!C13</f>
-        <v>DE90214500000105491377</v>
+        <v>0</v>
       </c>
       <c r="H4" s="44"/>
       <c r="I4" s="45"/>
       <c r="J4" s="45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="46"/>
       <c r="P4" s="99"/>
@@ -1807,41 +1783,41 @@
       <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="110" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="108" t="s">
+      <c r="B6" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="109"/>
-      <c r="H6" s="108" t="s">
+      <c r="G6" s="114"/>
+      <c r="H6" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
       <c r="K6" s="98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P6" s="99"/>
       <c r="Q6" s="100"/>
     </row>
     <row r="7" spans="1:17" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="109"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
+      <c r="A7" s="114"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
       <c r="K7" s="98" t="s">
         <v>4</v>
       </c>
@@ -1849,308 +1825,308 @@
       <c r="Q7" s="100"/>
     </row>
     <row r="8" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="135"/>
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="131"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="102"/>
       <c r="F8" s="96"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="131"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="102"/>
       <c r="M8" s="99"/>
       <c r="N8" s="100"/>
     </row>
     <row r="9" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="135"/>
-      <c r="B9" s="132"/>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="131"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="102"/>
       <c r="F9" s="96"/>
-      <c r="G9" s="131"/>
-      <c r="H9" s="133"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="134"/>
-      <c r="K9" s="131"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="102"/>
       <c r="M9" s="99"/>
       <c r="N9" s="100"/>
     </row>
     <row r="10" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="135"/>
-      <c r="B10" s="132"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="131"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="102"/>
       <c r="F10" s="96"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="134"/>
-      <c r="K10" s="131"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="102"/>
       <c r="M10" s="99"/>
       <c r="N10" s="100"/>
     </row>
     <row r="11" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="135"/>
-      <c r="B11" s="132"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="131"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="102"/>
       <c r="F11" s="96"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="133"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="134"/>
-      <c r="K11" s="131"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="102"/>
       <c r="M11" s="99"/>
       <c r="N11" s="100"/>
     </row>
     <row r="12" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="135"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="131"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="102"/>
       <c r="F12" s="96"/>
-      <c r="G12" s="131"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="134"/>
-      <c r="J12" s="134"/>
-      <c r="K12" s="131"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="102"/>
       <c r="M12" s="99"/>
       <c r="N12" s="100"/>
     </row>
     <row r="13" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="135"/>
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="131"/>
+      <c r="A13" s="103"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="102"/>
       <c r="F13" s="96"/>
-      <c r="G13" s="131"/>
-      <c r="H13" s="133"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="134"/>
-      <c r="K13" s="131"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="102"/>
       <c r="M13" s="99"/>
       <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="135"/>
-      <c r="B14" s="132"/>
-      <c r="C14" s="132"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="131"/>
+      <c r="A14" s="103"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="102"/>
       <c r="F14" s="96"/>
-      <c r="G14" s="131"/>
-      <c r="H14" s="133"/>
-      <c r="I14" s="134"/>
-      <c r="J14" s="134"/>
-      <c r="K14" s="131"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+      <c r="K14" s="102"/>
       <c r="M14" s="99"/>
       <c r="N14" s="100"/>
     </row>
     <row r="15" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="135"/>
-      <c r="B15" s="132"/>
-      <c r="C15" s="132"/>
-      <c r="D15" s="132"/>
-      <c r="E15" s="131"/>
+      <c r="A15" s="103"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="102"/>
       <c r="F15" s="96"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="133"/>
-      <c r="I15" s="134"/>
-      <c r="J15" s="134"/>
-      <c r="K15" s="131"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="111"/>
+      <c r="K15" s="102"/>
       <c r="M15" s="99"/>
       <c r="N15" s="100"/>
     </row>
     <row r="16" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="135"/>
-      <c r="B16" s="132"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="131"/>
+      <c r="A16" s="103"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="102"/>
       <c r="F16" s="96"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="134"/>
-      <c r="J16" s="134"/>
-      <c r="K16" s="131"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="111"/>
+      <c r="K16" s="102"/>
       <c r="M16" s="99"/>
       <c r="N16" s="100"/>
     </row>
     <row r="17" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="135"/>
-      <c r="B17" s="132"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="131"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="102"/>
       <c r="F17" s="96"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="134"/>
-      <c r="J17" s="134"/>
-      <c r="K17" s="131"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+      <c r="K17" s="102"/>
     </row>
     <row r="18" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="135"/>
-      <c r="B18" s="132"/>
-      <c r="C18" s="132"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="131"/>
+      <c r="A18" s="103"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="102"/>
       <c r="F18" s="96"/>
-      <c r="G18" s="131"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="134"/>
-      <c r="J18" s="134"/>
-      <c r="K18" s="131"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="111"/>
+      <c r="K18" s="102"/>
     </row>
     <row r="19" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="135"/>
-      <c r="B19" s="132"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="131"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="102"/>
       <c r="F19" s="96"/>
-      <c r="G19" s="131"/>
-      <c r="H19" s="133"/>
-      <c r="I19" s="134"/>
-      <c r="J19" s="134"/>
-      <c r="K19" s="131"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
+      <c r="K19" s="102"/>
     </row>
     <row r="20" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="135"/>
-      <c r="B20" s="132"/>
-      <c r="C20" s="132"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="131"/>
+      <c r="A20" s="103"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="102"/>
       <c r="F20" s="96"/>
-      <c r="G20" s="131"/>
-      <c r="H20" s="133"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="134"/>
-      <c r="K20" s="131"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="111"/>
+      <c r="K20" s="102"/>
     </row>
     <row r="21" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="135"/>
-      <c r="B21" s="132"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="131"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="102"/>
       <c r="F21" s="96"/>
-      <c r="G21" s="131"/>
-      <c r="H21" s="133"/>
-      <c r="I21" s="134"/>
-      <c r="J21" s="134"/>
-      <c r="K21" s="131"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="102"/>
     </row>
     <row r="22" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="135"/>
-      <c r="B22" s="132"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="132"/>
-      <c r="E22" s="131"/>
+      <c r="A22" s="103"/>
+      <c r="B22" s="96"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="102"/>
       <c r="F22" s="96"/>
-      <c r="G22" s="131"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="134"/>
-      <c r="J22" s="134"/>
-      <c r="K22" s="131"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
+      <c r="K22" s="102"/>
     </row>
     <row r="23" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="135"/>
-      <c r="B23" s="132"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="132"/>
-      <c r="E23" s="131"/>
+      <c r="A23" s="103"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="102"/>
       <c r="F23" s="96"/>
-      <c r="G23" s="131"/>
-      <c r="H23" s="133"/>
-      <c r="I23" s="134"/>
-      <c r="J23" s="134"/>
-      <c r="K23" s="131"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="110"/>
+      <c r="I23" s="111"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="102"/>
     </row>
     <row r="24" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="135"/>
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="131"/>
+      <c r="A24" s="103"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="102"/>
       <c r="F24" s="96"/>
-      <c r="G24" s="131"/>
-      <c r="H24" s="133"/>
-      <c r="I24" s="134"/>
-      <c r="J24" s="134"/>
-      <c r="K24" s="131"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="110"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="102"/>
     </row>
     <row r="25" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="135"/>
-      <c r="B25" s="132"/>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="131"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="102"/>
       <c r="F25" s="96"/>
-      <c r="G25" s="131"/>
-      <c r="H25" s="133"/>
-      <c r="I25" s="134"/>
-      <c r="J25" s="134"/>
-      <c r="K25" s="131"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="111"/>
+      <c r="J25" s="111"/>
+      <c r="K25" s="102"/>
     </row>
     <row r="26" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="135"/>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="131"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="102"/>
       <c r="F26" s="96"/>
-      <c r="G26" s="131"/>
-      <c r="H26" s="133"/>
-      <c r="I26" s="134"/>
-      <c r="J26" s="134"/>
-      <c r="K26" s="131"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="111"/>
+      <c r="J26" s="111"/>
+      <c r="K26" s="102"/>
     </row>
     <row r="27" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="135"/>
-      <c r="B27" s="132"/>
-      <c r="C27" s="132"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="131"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="102"/>
       <c r="F27" s="96"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="133"/>
-      <c r="I27" s="134"/>
-      <c r="J27" s="134"/>
-      <c r="K27" s="131"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="111"/>
+      <c r="J27" s="111"/>
+      <c r="K27" s="102"/>
     </row>
     <row r="28" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="135"/>
-      <c r="B28" s="132"/>
-      <c r="C28" s="132"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="131"/>
+      <c r="A28" s="103"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="102"/>
       <c r="F28" s="96"/>
-      <c r="G28" s="131"/>
-      <c r="H28" s="133"/>
-      <c r="I28" s="134"/>
-      <c r="J28" s="134"/>
-      <c r="K28" s="131"/>
+      <c r="G28" s="102"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="111"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="102"/>
     </row>
     <row r="29" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="135"/>
-      <c r="B29" s="132"/>
-      <c r="C29" s="132"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="131"/>
+      <c r="A29" s="103"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="102"/>
       <c r="F29" s="96"/>
-      <c r="G29" s="131"/>
-      <c r="H29" s="133"/>
-      <c r="I29" s="134"/>
-      <c r="J29" s="134"/>
-      <c r="K29" s="131"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="110"/>
+      <c r="I29" s="111"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="102"/>
     </row>
     <row r="30" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="95"/>
@@ -2232,10 +2208,10 @@
       <c r="C36" s="70"/>
       <c r="D36" s="41"/>
       <c r="E36" s="79" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F36" s="81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G36" s="59"/>
       <c r="H36" s="41"/>
@@ -2289,13 +2265,10 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="27">
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H9:J9"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:E7"/>
     <mergeCell ref="F6:G7"/>
@@ -2312,10 +2285,13 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2338,7 +2314,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2362,19 +2338,19 @@
     </row>
     <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="74"/>
       <c r="C2" s="52"/>
       <c r="D2" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="113" t="str">
+      <c r="E2" s="117">
         <f>Vorlage!C11</f>
-        <v>Pastor Simon Luthe</v>
-      </c>
-      <c r="F2" s="114"/>
-      <c r="G2" s="115"/>
+        <v>0</v>
+      </c>
+      <c r="F2" s="118"/>
+      <c r="G2" s="119"/>
     </row>
     <row r="3" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="65"/>
@@ -2389,20 +2365,20 @@
       <c r="A4" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="56" t="str">
+      <c r="B4" s="56">
         <f>Vorlage!C7</f>
-        <v>Kirchengemeinde Wesselburen</v>
+        <v>0</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="116" t="str">
+      <c r="E4" s="120">
         <f>Vorlage!C12</f>
-        <v>Süderstr. 18, 25779 Hennstedt</v>
-      </c>
-      <c r="F4" s="117"/>
-      <c r="G4" s="118"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="121"/>
+      <c r="G4" s="122"/>
     </row>
     <row r="5" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="65"/>
@@ -2418,36 +2394,36 @@
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="128" t="str">
+        <v>23</v>
+      </c>
+      <c r="E6" s="132">
         <f>Vorlage!C13</f>
-        <v>DE90214500000105491377</v>
-      </c>
-      <c r="F6" s="129"/>
-      <c r="G6" s="130"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="133"/>
+      <c r="G6" s="134"/>
     </row>
     <row r="7" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="123" t="s">
+      <c r="C8" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="124"/>
-      <c r="E8" s="125" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="126"/>
-      <c r="G8" s="127"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="129" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="130"/>
+      <c r="G8" s="131"/>
     </row>
     <row r="9" spans="1:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="120"/>
-      <c r="B9" s="122"/>
+      <c r="A9" s="124"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -2607,7 +2583,10 @@
       <c r="F25" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="39"/>
+      <c r="G25" s="39">
+        <f>SUM(G10:G24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
@@ -2633,18 +2612,19 @@
         <v>2</v>
       </c>
       <c r="B28" s="77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="53"/>
       <c r="E28" s="78"/>
       <c r="F28" s="91" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="92" t="s">
-        <v>22</v>
+        <v>37</v>
+      </c>
+      <c r="G28" s="92">
+        <f>G25*0.05</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="14" thickTop="1" x14ac:dyDescent="0.15">
@@ -2670,13 +2650,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="93" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" s="94" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="62"/>
       <c r="F31" s="62"/>

</xml_diff>

<commit_message>
reperatur bearbeiten hinzufügen mitfahrer in fahrtenliste
</commit_message>
<xml_diff>
--- a/backend/templates/fahrtenabrechnung_vorlage.xlsx
+++ b/backend/templates/fahrtenabrechnung_vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonluthe/Documents/Fahrtenbuch/backend/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C7BC20-D74D-2243-8F40-DACE9773604D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDCD9CC-B219-B040-8225-B304EF986AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{F46B887E-D2C8-3347-9EF3-8F9C6453CC26}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" activeTab="2" xr2:uid="{F46B887E-D2C8-3347-9EF3-8F9C6453CC26}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="1" r:id="rId1"/>
@@ -911,7 +911,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -938,22 +938,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1133,6 +1127,9 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1145,9 +1142,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1202,7 +1196,24 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -1534,32 +1545,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="29"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
@@ -1568,7 +1579,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="36"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
@@ -1577,7 +1588,7 @@
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
-      <c r="D8" s="34"/>
+      <c r="D8" s="28"/>
       <c r="J8" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1585,61 +1596,61 @@
         <v>6</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
     </row>
     <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
     </row>
     <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
       <c r="G13" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
@@ -1684,7 +1695,7 @@
   </sheetPr>
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1708,426 +1719,426 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52">
+      <c r="G2" s="46">
         <f>Vorlage!C11</f>
         <v>0</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="53"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:17" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="49">
         <f>Vorlage!C7</f>
         <v>0</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="58">
+      <c r="G3" s="52">
         <f>Vorlage!C12</f>
         <v>0</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="59"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="99"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="53"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="93"/>
     </row>
     <row r="4" spans="1:17" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="42" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="37">
         <f>Vorlage!C13</f>
         <v>0</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45" t="s">
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="99"/>
+      <c r="K4" s="40"/>
+      <c r="P4" s="92"/>
+      <c r="Q4" s="93"/>
     </row>
     <row r="5" spans="1:17" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J5" s="6"/>
       <c r="K5" s="5"/>
-      <c r="P5" s="98"/>
-      <c r="Q5" s="99"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="93"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="111" t="s">
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="111" t="s">
+      <c r="G6" s="107"/>
+      <c r="H6" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="97" t="s">
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="98"/>
-      <c r="Q6" s="99"/>
+      <c r="P6" s="92"/>
+      <c r="Q6" s="93"/>
     </row>
     <row r="7" spans="1:17" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="112"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="97" t="s">
+      <c r="A7" s="107"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="99"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="93"/>
     </row>
     <row r="8" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="102"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="101"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="99"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="95"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="93"/>
     </row>
     <row r="9" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="102"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="101"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="99"/>
+      <c r="A9" s="96"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="95"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="102"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
-      <c r="K10" s="101"/>
-      <c r="M10" s="98"/>
-      <c r="N10" s="99"/>
+      <c r="A10" s="96"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="95"/>
+      <c r="M10" s="92"/>
+      <c r="N10" s="93"/>
     </row>
     <row r="11" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="102"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="101"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="99"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="95"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="93"/>
     </row>
     <row r="12" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="102"/>
-      <c r="B12" s="95"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
-      <c r="K12" s="101"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="99"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="95"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="93"/>
     </row>
     <row r="13" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="102"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="101"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="99"/>
+      <c r="A13" s="96"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="95"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="93"/>
     </row>
     <row r="14" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="102"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="101"/>
-      <c r="M14" s="98"/>
-      <c r="N14" s="99"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="95"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="93"/>
     </row>
     <row r="15" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="102"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="101"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="99"/>
+      <c r="A15" s="96"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="95"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="93"/>
     </row>
     <row r="16" spans="1:17" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="102"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="110"/>
-      <c r="K16" s="101"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="99"/>
+      <c r="A16" s="96"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="95"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="93"/>
     </row>
     <row r="17" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="102"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="110"/>
-      <c r="K17" s="101"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="95"/>
     </row>
     <row r="18" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="102"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="110"/>
-      <c r="K18" s="101"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="95"/>
     </row>
     <row r="19" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="102"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="101"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="95"/>
     </row>
     <row r="20" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="102"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="109"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="101"/>
+      <c r="A20" s="96"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="103"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="95"/>
     </row>
     <row r="21" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="102"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="101"/>
+      <c r="A21" s="96"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="95"/>
     </row>
     <row r="22" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="102"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="101"/>
+      <c r="A22" s="96"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="103"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="95"/>
     </row>
     <row r="23" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="102"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="101"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="95"/>
     </row>
     <row r="24" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="102"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="110"/>
-      <c r="K24" s="101"/>
+      <c r="A24" s="96"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="95"/>
     </row>
     <row r="25" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="102"/>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="101"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="110"/>
-      <c r="K25" s="101"/>
+      <c r="A25" s="96"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="95"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="95"/>
     </row>
     <row r="26" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="102"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="101"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="110"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="101"/>
+      <c r="A26" s="96"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="95"/>
     </row>
     <row r="27" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="102"/>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="101"/>
+      <c r="A27" s="96"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="95"/>
     </row>
     <row r="28" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="102"/>
-      <c r="B28" s="95"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="109"/>
-      <c r="I28" s="110"/>
-      <c r="J28" s="110"/>
-      <c r="K28" s="101"/>
+      <c r="A28" s="96"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="95"/>
     </row>
     <row r="29" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="102"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="101"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="95"/>
     </row>
     <row r="30" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="94"/>
+      <c r="A30" s="88"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2135,141 +2146,144 @@
       <c r="J30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K30" s="96">
+      <c r="K30" s="90">
         <f>SUM(K8:K29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="94"/>
+      <c r="A31" s="88"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="94"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:11" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
-      <c r="B33" s="115"/>
-      <c r="C33" s="115"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="82" t="s">
+      <c r="A33" s="88"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="83" t="s">
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="K33" s="100">
+      <c r="K33" s="94">
         <f>K30*0.3</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="94"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="66"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="60"/>
     </row>
     <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="94"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="68"/>
+      <c r="A35" s="88"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="62"/>
     </row>
     <row r="36" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="94"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="78" t="s">
+      <c r="A36" s="88"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="80" t="s">
+      <c r="F36" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="G36" s="58"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="70"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="64"/>
     </row>
     <row r="37" spans="1:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="94"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="71"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="72"/>
+      <c r="A37" s="88"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="66"/>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="94"/>
+      <c r="A38" s="88"/>
     </row>
     <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="94"/>
+      <c r="A52" s="88"/>
     </row>
     <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="94"/>
+      <c r="A53" s="88"/>
     </row>
     <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="94"/>
+      <c r="A54" s="88"/>
     </row>
     <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="94"/>
+      <c r="A55" s="88"/>
     </row>
     <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="94"/>
+      <c r="A56" s="88"/>
     </row>
     <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="94"/>
+      <c r="A57" s="88"/>
     </row>
     <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="94"/>
+      <c r="A58" s="88"/>
     </row>
     <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="94"/>
+      <c r="A59" s="88"/>
     </row>
     <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="94"/>
+      <c r="A60" s="88"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="27">
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:E7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="H6:J7"/>
+    <mergeCell ref="H8:J8"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H14:J14"/>
@@ -2280,16 +2294,13 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:E7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="H6:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2311,8 +2322,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2335,93 +2346,93 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="85" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="116">
+      <c r="E2" s="110">
         <f>Vorlage!C11</f>
         <v>0</v>
       </c>
-      <c r="F2" s="117"/>
-      <c r="G2" s="118"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="112"/>
     </row>
     <row r="3" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="64"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="86"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="49">
         <f>Vorlage!C7</f>
         <v>0</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="56" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="119">
+      <c r="E4" s="113">
         <f>Vorlage!C12</f>
         <v>0</v>
       </c>
-      <c r="F4" s="120"/>
-      <c r="G4" s="121"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="115"/>
     </row>
     <row r="5" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="64"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="89"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="83"/>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="75"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="62" t="s">
+      <c r="A6" s="69"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="131">
+      <c r="E6" s="125">
         <f>Vorlage!C13</f>
         <v>0</v>
       </c>
-      <c r="F6" s="132"/>
-      <c r="G6" s="133"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="127"/>
     </row>
     <row r="7" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="124" t="s">
+      <c r="B8" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="126" t="s">
+      <c r="C8" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="127"/>
-      <c r="E8" s="128" t="s">
+      <c r="D8" s="121"/>
+      <c r="E8" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="129"/>
-      <c r="G8" s="130"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
     </row>
     <row r="9" spans="1:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="123"/>
-      <c r="B9" s="125"/>
+      <c r="A9" s="117"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -2431,157 +2442,157 @@
       <c r="E9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="26"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="27"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="27"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="27"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="27"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="27"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="27"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="130"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="27"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="27"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="19" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="27"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="27"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="27"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="21"/>
     </row>
     <row r="22" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="27"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="131"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="27"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="28"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="22"/>
     </row>
     <row r="25" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="33">
         <f>SUM(G10:G24)</f>
         <v>0</v>
       </c>
@@ -2606,67 +2617,67 @@
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="52"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="90" t="s">
+      <c r="D28" s="46"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="91">
+      <c r="G28" s="85">
         <f>G25*0.05</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="14" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="41"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="66"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="60"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="68"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="62"/>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="92" t="s">
+      <c r="C31" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="93" t="s">
+      <c r="D31" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="72"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="66"/>
     </row>
     <row r="32" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>